<commit_message>
READY_FOR_SPELLING becomes USE_SPELLING, constructed mechanism to cycle on S for generation of data
</commit_message>
<xml_diff>
--- a/data_collection/adjusted/adjusted_recap.xlsx
+++ b/data_collection/adjusted/adjusted_recap.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="18">
   <si>
     <t>DIALOGUE 1</t>
   </si>
@@ -41,6 +41,18 @@
   </si>
   <si>
     <t>DIALOGUE 8</t>
+  </si>
+  <si>
+    <t>DIALOGUE 9</t>
+  </si>
+  <si>
+    <t>DIALOGUE 10</t>
+  </si>
+  <si>
+    <t>DIALOGUE 11</t>
+  </si>
+  <si>
+    <t>DIALOGUE 12</t>
   </si>
   <si>
     <t>S = 2</t>
@@ -387,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A5:AC66"/>
+  <dimension ref="A5:AC98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -404,31 +416,31 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K5" t="s">
         <v>0</v>
       </c>
       <c r="M5" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="P5" t="s">
         <v>0</v>
       </c>
       <c r="R5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="U5" t="s">
         <v>0</v>
       </c>
       <c r="W5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Z5" t="s">
         <v>0</v>
       </c>
       <c r="AB5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:29">
@@ -812,31 +824,31 @@
         <v>2</v>
       </c>
       <c r="H13" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K13" t="s">
         <v>2</v>
       </c>
       <c r="M13" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="P13" t="s">
         <v>2</v>
       </c>
       <c r="R13" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="U13" t="s">
         <v>2</v>
       </c>
       <c r="W13" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Z13" t="s">
         <v>2</v>
       </c>
       <c r="AB13" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:29">
@@ -1220,31 +1232,31 @@
         <v>3</v>
       </c>
       <c r="H21" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K21" t="s">
         <v>3</v>
       </c>
       <c r="M21" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="P21" t="s">
         <v>3</v>
       </c>
       <c r="R21" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="U21" t="s">
         <v>3</v>
       </c>
       <c r="W21" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Z21" t="s">
         <v>3</v>
       </c>
       <c r="AB21" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:29">
@@ -1628,31 +1640,31 @@
         <v>4</v>
       </c>
       <c r="H29" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K29" t="s">
         <v>4</v>
       </c>
       <c r="M29" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="P29" t="s">
         <v>4</v>
       </c>
       <c r="R29" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="U29" t="s">
         <v>4</v>
       </c>
       <c r="W29" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Z29" t="s">
         <v>4</v>
       </c>
       <c r="AB29" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:29">
@@ -2036,31 +2048,31 @@
         <v>5</v>
       </c>
       <c r="H37" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K37" t="s">
         <v>5</v>
       </c>
       <c r="M37" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="P37" t="s">
         <v>5</v>
       </c>
       <c r="R37" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="U37" t="s">
         <v>5</v>
       </c>
       <c r="W37" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Z37" t="s">
         <v>5</v>
       </c>
       <c r="AB37" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:29">
@@ -2444,31 +2456,31 @@
         <v>6</v>
       </c>
       <c r="H45" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K45" t="s">
         <v>6</v>
       </c>
       <c r="M45" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="P45" t="s">
         <v>6</v>
       </c>
       <c r="R45" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="U45" t="s">
         <v>6</v>
       </c>
       <c r="W45" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Z45" t="s">
         <v>6</v>
       </c>
       <c r="AB45" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:29">
@@ -2852,31 +2864,31 @@
         <v>7</v>
       </c>
       <c r="H53" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K53" t="s">
         <v>7</v>
       </c>
       <c r="M53" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="P53" t="s">
         <v>7</v>
       </c>
       <c r="R53" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="U53" t="s">
         <v>7</v>
       </c>
       <c r="W53" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Z53" t="s">
         <v>7</v>
       </c>
       <c r="AB53" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:29">
@@ -3260,31 +3272,31 @@
         <v>8</v>
       </c>
       <c r="H61" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K61" t="s">
         <v>8</v>
       </c>
       <c r="M61" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="P61" t="s">
         <v>8</v>
       </c>
       <c r="R61" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="U61" t="s">
         <v>8</v>
       </c>
       <c r="W61" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Z61" t="s">
         <v>8</v>
       </c>
       <c r="AB61" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:29">
@@ -3655,6 +3667,1638 @@
       </c>
       <c r="AC66">
         <v>19</v>
+      </c>
+    </row>
+    <row r="69" spans="1:29">
+      <c r="A69" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" t="s">
+        <v>1</v>
+      </c>
+      <c r="F69" t="s">
+        <v>9</v>
+      </c>
+      <c r="H69" t="s">
+        <v>13</v>
+      </c>
+      <c r="K69" t="s">
+        <v>9</v>
+      </c>
+      <c r="M69" t="s">
+        <v>14</v>
+      </c>
+      <c r="P69" t="s">
+        <v>9</v>
+      </c>
+      <c r="R69" t="s">
+        <v>15</v>
+      </c>
+      <c r="U69" t="s">
+        <v>9</v>
+      </c>
+      <c r="W69" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z69" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB69" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="70" spans="1:29">
+      <c r="A70">
+        <v>1.5</v>
+      </c>
+      <c r="B70">
+        <v>27</v>
+      </c>
+      <c r="C70">
+        <v>0.88</v>
+      </c>
+      <c r="D70">
+        <v>23</v>
+      </c>
+      <c r="F70">
+        <v>1.88</v>
+      </c>
+      <c r="G70">
+        <v>30</v>
+      </c>
+      <c r="H70">
+        <v>0.71</v>
+      </c>
+      <c r="I70">
+        <v>23</v>
+      </c>
+      <c r="K70">
+        <v>1.71</v>
+      </c>
+      <c r="L70">
+        <v>36</v>
+      </c>
+      <c r="M70">
+        <v>0.79</v>
+      </c>
+      <c r="N70">
+        <v>27</v>
+      </c>
+      <c r="P70">
+        <v>2.59</v>
+      </c>
+      <c r="Q70">
+        <v>44</v>
+      </c>
+      <c r="R70">
+        <v>0.88</v>
+      </c>
+      <c r="S70">
+        <v>22</v>
+      </c>
+      <c r="U70">
+        <v>1.93</v>
+      </c>
+      <c r="V70">
+        <v>27</v>
+      </c>
+      <c r="W70">
+        <v>1</v>
+      </c>
+      <c r="X70">
+        <v>18</v>
+      </c>
+      <c r="Z70">
+        <v>1.38</v>
+      </c>
+      <c r="AA70">
+        <v>47</v>
+      </c>
+      <c r="AB70">
+        <v>0.31</v>
+      </c>
+      <c r="AC70">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="71" spans="1:29">
+      <c r="A71">
+        <v>1.47</v>
+      </c>
+      <c r="B71">
+        <v>25</v>
+      </c>
+      <c r="C71">
+        <v>0.85</v>
+      </c>
+      <c r="D71">
+        <v>22</v>
+      </c>
+      <c r="F71">
+        <v>1.7</v>
+      </c>
+      <c r="G71">
+        <v>34</v>
+      </c>
+      <c r="H71">
+        <v>0.52</v>
+      </c>
+      <c r="I71">
+        <v>29</v>
+      </c>
+      <c r="K71">
+        <v>1.71</v>
+      </c>
+      <c r="L71">
+        <v>29</v>
+      </c>
+      <c r="M71">
+        <v>0.85</v>
+      </c>
+      <c r="N71">
+        <v>22</v>
+      </c>
+      <c r="P71">
+        <v>1.88</v>
+      </c>
+      <c r="Q71">
+        <v>32</v>
+      </c>
+      <c r="R71">
+        <v>0.85</v>
+      </c>
+      <c r="S71">
+        <v>22</v>
+      </c>
+      <c r="U71">
+        <v>1.47</v>
+      </c>
+      <c r="V71">
+        <v>28</v>
+      </c>
+      <c r="W71">
+        <v>0.73</v>
+      </c>
+      <c r="X71">
+        <v>25</v>
+      </c>
+      <c r="Z71">
+        <v>1.76</v>
+      </c>
+      <c r="AA71">
+        <v>30</v>
+      </c>
+      <c r="AB71">
+        <v>0.85</v>
+      </c>
+      <c r="AC71">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="72" spans="1:29">
+      <c r="A72">
+        <v>2.33</v>
+      </c>
+      <c r="B72">
+        <v>14</v>
+      </c>
+      <c r="C72">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="D72">
+        <v>13</v>
+      </c>
+      <c r="F72">
+        <v>5</v>
+      </c>
+      <c r="G72">
+        <v>35</v>
+      </c>
+      <c r="H72">
+        <v>0.6</v>
+      </c>
+      <c r="I72">
+        <v>15</v>
+      </c>
+      <c r="K72">
+        <v>4.62</v>
+      </c>
+      <c r="L72">
+        <v>37</v>
+      </c>
+      <c r="M72">
+        <v>0.53</v>
+      </c>
+      <c r="N72">
+        <v>17</v>
+      </c>
+      <c r="P72">
+        <v>2.33</v>
+      </c>
+      <c r="Q72">
+        <v>14</v>
+      </c>
+      <c r="R72">
+        <v>0.82</v>
+      </c>
+      <c r="S72">
+        <v>12</v>
+      </c>
+      <c r="U72">
+        <v>5</v>
+      </c>
+      <c r="V72">
+        <v>30</v>
+      </c>
+      <c r="W72">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="X72">
+        <v>13</v>
+      </c>
+      <c r="Z72">
+        <v>2.4</v>
+      </c>
+      <c r="AA72">
+        <v>12</v>
+      </c>
+      <c r="AB72">
+        <v>0.82</v>
+      </c>
+      <c r="AC72">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="73" spans="1:29">
+      <c r="A73">
+        <v>1.35</v>
+      </c>
+      <c r="B73">
+        <v>69</v>
+      </c>
+      <c r="C73">
+        <v>0.91</v>
+      </c>
+      <c r="D73">
+        <v>65</v>
+      </c>
+      <c r="F73">
+        <v>1.71</v>
+      </c>
+      <c r="G73">
+        <v>96</v>
+      </c>
+      <c r="H73">
+        <v>0.83</v>
+      </c>
+      <c r="I73">
+        <v>72</v>
+      </c>
+      <c r="K73">
+        <v>1.69</v>
+      </c>
+      <c r="L73">
+        <v>98</v>
+      </c>
+      <c r="M73">
+        <v>0.91</v>
+      </c>
+      <c r="N73">
+        <v>72</v>
+      </c>
+      <c r="P73">
+        <v>1.77</v>
+      </c>
+      <c r="Q73">
+        <v>92</v>
+      </c>
+      <c r="R73">
+        <v>1</v>
+      </c>
+      <c r="S73">
+        <v>64</v>
+      </c>
+      <c r="U73">
+        <v>1.62</v>
+      </c>
+      <c r="V73">
+        <v>91</v>
+      </c>
+      <c r="W73">
+        <v>0.91</v>
+      </c>
+      <c r="X73">
+        <v>70</v>
+      </c>
+      <c r="Z73">
+        <v>1.81</v>
+      </c>
+      <c r="AA73">
+        <v>96</v>
+      </c>
+      <c r="AB73">
+        <v>0.87</v>
+      </c>
+      <c r="AC73">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="74" spans="1:29">
+      <c r="A74">
+        <v>2.09</v>
+      </c>
+      <c r="B74">
+        <v>23</v>
+      </c>
+      <c r="C74">
+        <v>0.87</v>
+      </c>
+      <c r="D74">
+        <v>17</v>
+      </c>
+      <c r="F74">
+        <v>1.8</v>
+      </c>
+      <c r="G74">
+        <v>27</v>
+      </c>
+      <c r="H74">
+        <v>0.68</v>
+      </c>
+      <c r="I74">
+        <v>23</v>
+      </c>
+      <c r="K74">
+        <v>1.82</v>
+      </c>
+      <c r="L74">
+        <v>20</v>
+      </c>
+      <c r="M74">
+        <v>0.87</v>
+      </c>
+      <c r="N74">
+        <v>17</v>
+      </c>
+      <c r="P74">
+        <v>1.92</v>
+      </c>
+      <c r="Q74">
+        <v>23</v>
+      </c>
+      <c r="R74">
+        <v>0.87</v>
+      </c>
+      <c r="S74">
+        <v>18</v>
+      </c>
+      <c r="U74">
+        <v>2.2</v>
+      </c>
+      <c r="V74">
+        <v>22</v>
+      </c>
+      <c r="W74">
+        <v>0.87</v>
+      </c>
+      <c r="X74">
+        <v>16</v>
+      </c>
+      <c r="Z74">
+        <v>1.93</v>
+      </c>
+      <c r="AA74">
+        <v>27</v>
+      </c>
+      <c r="AB74">
+        <v>0.87</v>
+      </c>
+      <c r="AC74">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="77" spans="1:29">
+      <c r="A77" t="s">
+        <v>10</v>
+      </c>
+      <c r="C77" t="s">
+        <v>1</v>
+      </c>
+      <c r="F77" t="s">
+        <v>10</v>
+      </c>
+      <c r="H77" t="s">
+        <v>13</v>
+      </c>
+      <c r="K77" t="s">
+        <v>10</v>
+      </c>
+      <c r="M77" t="s">
+        <v>14</v>
+      </c>
+      <c r="P77" t="s">
+        <v>10</v>
+      </c>
+      <c r="R77" t="s">
+        <v>15</v>
+      </c>
+      <c r="U77" t="s">
+        <v>10</v>
+      </c>
+      <c r="W77" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z77" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB77" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="78" spans="1:29">
+      <c r="A78">
+        <v>1.81</v>
+      </c>
+      <c r="B78">
+        <v>29</v>
+      </c>
+      <c r="C78">
+        <v>0.79</v>
+      </c>
+      <c r="D78">
+        <v>22</v>
+      </c>
+      <c r="F78">
+        <v>1.81</v>
+      </c>
+      <c r="G78">
+        <v>38</v>
+      </c>
+      <c r="H78">
+        <v>0.71</v>
+      </c>
+      <c r="I78">
+        <v>28</v>
+      </c>
+      <c r="K78">
+        <v>1.53</v>
+      </c>
+      <c r="L78">
+        <v>23</v>
+      </c>
+      <c r="M78">
+        <v>0.88</v>
+      </c>
+      <c r="N78">
+        <v>20</v>
+      </c>
+      <c r="P78">
+        <v>1.8</v>
+      </c>
+      <c r="Q78">
+        <v>27</v>
+      </c>
+      <c r="R78">
+        <v>0.88</v>
+      </c>
+      <c r="S78">
+        <v>20</v>
+      </c>
+      <c r="U78">
+        <v>1.44</v>
+      </c>
+      <c r="V78">
+        <v>23</v>
+      </c>
+      <c r="W78">
+        <v>0.88</v>
+      </c>
+      <c r="X78">
+        <v>21</v>
+      </c>
+      <c r="Z78">
+        <v>1.9</v>
+      </c>
+      <c r="AA78">
+        <v>38</v>
+      </c>
+      <c r="AB78">
+        <v>0.79</v>
+      </c>
+      <c r="AC78">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="79" spans="1:29">
+      <c r="A79">
+        <v>1.81</v>
+      </c>
+      <c r="B79">
+        <v>29</v>
+      </c>
+      <c r="C79">
+        <v>0.85</v>
+      </c>
+      <c r="D79">
+        <v>21</v>
+      </c>
+      <c r="F79">
+        <v>1.59</v>
+      </c>
+      <c r="G79">
+        <v>43</v>
+      </c>
+      <c r="H79">
+        <v>0.41</v>
+      </c>
+      <c r="I79">
+        <v>39</v>
+      </c>
+      <c r="K79">
+        <v>1.79</v>
+      </c>
+      <c r="L79">
+        <v>34</v>
+      </c>
+      <c r="M79">
+        <v>0.65</v>
+      </c>
+      <c r="N79">
+        <v>26</v>
+      </c>
+      <c r="P79">
+        <v>1.71</v>
+      </c>
+      <c r="Q79">
+        <v>29</v>
+      </c>
+      <c r="R79">
+        <v>0.85</v>
+      </c>
+      <c r="S79">
+        <v>22</v>
+      </c>
+      <c r="U79">
+        <v>1.71</v>
+      </c>
+      <c r="V79">
+        <v>29</v>
+      </c>
+      <c r="W79">
+        <v>0.85</v>
+      </c>
+      <c r="X79">
+        <v>22</v>
+      </c>
+      <c r="Z79">
+        <v>2</v>
+      </c>
+      <c r="AA79">
+        <v>34</v>
+      </c>
+      <c r="AB79">
+        <v>0.85</v>
+      </c>
+      <c r="AC79">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="80" spans="1:29">
+      <c r="A80">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="B80">
+        <v>41</v>
+      </c>
+      <c r="C80">
+        <v>0.82</v>
+      </c>
+      <c r="D80">
+        <v>11</v>
+      </c>
+      <c r="F80">
+        <v>4.33</v>
+      </c>
+      <c r="G80">
+        <v>39</v>
+      </c>
+      <c r="H80">
+        <v>0.47</v>
+      </c>
+      <c r="I80">
+        <v>19</v>
+      </c>
+      <c r="K80">
+        <v>5</v>
+      </c>
+      <c r="L80">
+        <v>35</v>
+      </c>
+      <c r="M80">
+        <v>0.6</v>
+      </c>
+      <c r="N80">
+        <v>15</v>
+      </c>
+      <c r="P80">
+        <v>3.67</v>
+      </c>
+      <c r="Q80">
+        <v>33</v>
+      </c>
+      <c r="R80">
+        <v>0.47</v>
+      </c>
+      <c r="S80">
+        <v>19</v>
+      </c>
+      <c r="U80">
+        <v>2.2</v>
+      </c>
+      <c r="V80">
+        <v>11</v>
+      </c>
+      <c r="W80">
+        <v>0.82</v>
+      </c>
+      <c r="X80">
+        <v>11</v>
+      </c>
+      <c r="Z80">
+        <v>5.8</v>
+      </c>
+      <c r="AA80">
+        <v>29</v>
+      </c>
+      <c r="AB80">
+        <v>0.82</v>
+      </c>
+      <c r="AC80">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="1:29">
+      <c r="A81">
+        <v>1.38</v>
+      </c>
+      <c r="B81">
+        <v>69</v>
+      </c>
+      <c r="C81">
+        <v>1</v>
+      </c>
+      <c r="D81">
+        <v>62</v>
+      </c>
+      <c r="F81">
+        <v>1.76</v>
+      </c>
+      <c r="G81">
+        <v>97</v>
+      </c>
+      <c r="H81">
+        <v>0.87</v>
+      </c>
+      <c r="I81">
+        <v>70</v>
+      </c>
+      <c r="K81">
+        <v>1.68</v>
+      </c>
+      <c r="L81">
+        <v>84</v>
+      </c>
+      <c r="M81">
+        <v>0.95</v>
+      </c>
+      <c r="N81">
+        <v>63</v>
+      </c>
+      <c r="P81">
+        <v>1.39</v>
+      </c>
+      <c r="Q81">
+        <v>82</v>
+      </c>
+      <c r="R81">
+        <v>0.95</v>
+      </c>
+      <c r="S81">
+        <v>72</v>
+      </c>
+      <c r="U81">
+        <v>1.62</v>
+      </c>
+      <c r="V81">
+        <v>104</v>
+      </c>
+      <c r="W81">
+        <v>0.95</v>
+      </c>
+      <c r="X81">
+        <v>77</v>
+      </c>
+      <c r="Z81">
+        <v>1.69</v>
+      </c>
+      <c r="AA81">
+        <v>105</v>
+      </c>
+      <c r="AB81">
+        <v>0.91</v>
+      </c>
+      <c r="AC81">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="82" spans="1:29">
+      <c r="A82">
+        <v>2.08</v>
+      </c>
+      <c r="B82">
+        <v>27</v>
+      </c>
+      <c r="C82">
+        <v>0.76</v>
+      </c>
+      <c r="D82">
+        <v>20</v>
+      </c>
+      <c r="F82">
+        <v>1.71</v>
+      </c>
+      <c r="G82">
+        <v>29</v>
+      </c>
+      <c r="H82">
+        <v>0.76</v>
+      </c>
+      <c r="I82">
+        <v>24</v>
+      </c>
+      <c r="K82">
+        <v>2.07</v>
+      </c>
+      <c r="L82">
+        <v>29</v>
+      </c>
+      <c r="M82">
+        <v>0.87</v>
+      </c>
+      <c r="N82">
+        <v>20</v>
+      </c>
+      <c r="P82">
+        <v>1.93</v>
+      </c>
+      <c r="Q82">
+        <v>29</v>
+      </c>
+      <c r="R82">
+        <v>0.87</v>
+      </c>
+      <c r="S82">
+        <v>21</v>
+      </c>
+      <c r="U82">
+        <v>1.57</v>
+      </c>
+      <c r="V82">
+        <v>22</v>
+      </c>
+      <c r="W82">
+        <v>0.87</v>
+      </c>
+      <c r="X82">
+        <v>20</v>
+      </c>
+      <c r="Z82">
+        <v>1.92</v>
+      </c>
+      <c r="AA82">
+        <v>25</v>
+      </c>
+      <c r="AB82">
+        <v>0.76</v>
+      </c>
+      <c r="AC82">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="85" spans="1:29">
+      <c r="A85" t="s">
+        <v>11</v>
+      </c>
+      <c r="C85" t="s">
+        <v>1</v>
+      </c>
+      <c r="F85" t="s">
+        <v>11</v>
+      </c>
+      <c r="H85" t="s">
+        <v>13</v>
+      </c>
+      <c r="K85" t="s">
+        <v>11</v>
+      </c>
+      <c r="M85" t="s">
+        <v>14</v>
+      </c>
+      <c r="P85" t="s">
+        <v>11</v>
+      </c>
+      <c r="R85" t="s">
+        <v>15</v>
+      </c>
+      <c r="U85" t="s">
+        <v>11</v>
+      </c>
+      <c r="W85" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z85" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB85" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="86" spans="1:29">
+      <c r="A86">
+        <v>1.94</v>
+      </c>
+      <c r="B86">
+        <v>33</v>
+      </c>
+      <c r="C86">
+        <v>0.88</v>
+      </c>
+      <c r="D86">
+        <v>22</v>
+      </c>
+      <c r="F86">
+        <v>1.4</v>
+      </c>
+      <c r="G86">
+        <v>28</v>
+      </c>
+      <c r="H86">
+        <v>0.71</v>
+      </c>
+      <c r="I86">
+        <v>27</v>
+      </c>
+      <c r="K86">
+        <v>1.63</v>
+      </c>
+      <c r="L86">
+        <v>31</v>
+      </c>
+      <c r="M86">
+        <v>0.88</v>
+      </c>
+      <c r="N86">
+        <v>24</v>
+      </c>
+      <c r="P86">
+        <v>1.89</v>
+      </c>
+      <c r="Q86">
+        <v>34</v>
+      </c>
+      <c r="R86">
+        <v>0.88</v>
+      </c>
+      <c r="S86">
+        <v>23</v>
+      </c>
+      <c r="U86">
+        <v>2.18</v>
+      </c>
+      <c r="V86">
+        <v>37</v>
+      </c>
+      <c r="W86">
+        <v>0.88</v>
+      </c>
+      <c r="X86">
+        <v>22</v>
+      </c>
+      <c r="Z86">
+        <v>1.85</v>
+      </c>
+      <c r="AA86">
+        <v>24</v>
+      </c>
+      <c r="AB86">
+        <v>0.88</v>
+      </c>
+      <c r="AC86">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87" spans="1:29">
+      <c r="A87">
+        <v>1.72</v>
+      </c>
+      <c r="B87">
+        <v>31</v>
+      </c>
+      <c r="C87">
+        <v>0.85</v>
+      </c>
+      <c r="D87">
+        <v>23</v>
+      </c>
+      <c r="F87">
+        <v>1.7</v>
+      </c>
+      <c r="G87">
+        <v>34</v>
+      </c>
+      <c r="H87">
+        <v>0.65</v>
+      </c>
+      <c r="I87">
+        <v>27</v>
+      </c>
+      <c r="K87">
+        <v>1.65</v>
+      </c>
+      <c r="L87">
+        <v>33</v>
+      </c>
+      <c r="M87">
+        <v>0.85</v>
+      </c>
+      <c r="N87">
+        <v>25</v>
+      </c>
+      <c r="P87">
+        <v>1.81</v>
+      </c>
+      <c r="Q87">
+        <v>29</v>
+      </c>
+      <c r="R87">
+        <v>0.85</v>
+      </c>
+      <c r="S87">
+        <v>21</v>
+      </c>
+      <c r="U87">
+        <v>1.71</v>
+      </c>
+      <c r="V87">
+        <v>29</v>
+      </c>
+      <c r="W87">
+        <v>1</v>
+      </c>
+      <c r="X87">
+        <v>21</v>
+      </c>
+      <c r="Z87">
+        <v>1.88</v>
+      </c>
+      <c r="AA87">
+        <v>32</v>
+      </c>
+      <c r="AB87">
+        <v>0.85</v>
+      </c>
+      <c r="AC87">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="88" spans="1:29">
+      <c r="A88">
+        <v>5.4</v>
+      </c>
+      <c r="B88">
+        <v>27</v>
+      </c>
+      <c r="C88">
+        <v>0.82</v>
+      </c>
+      <c r="D88">
+        <v>11</v>
+      </c>
+      <c r="F88">
+        <v>1.73</v>
+      </c>
+      <c r="G88">
+        <v>19</v>
+      </c>
+      <c r="H88">
+        <v>0.39</v>
+      </c>
+      <c r="I88">
+        <v>23</v>
+      </c>
+      <c r="K88">
+        <v>5</v>
+      </c>
+      <c r="L88">
+        <v>35</v>
+      </c>
+      <c r="M88">
+        <v>0.6</v>
+      </c>
+      <c r="N88">
+        <v>15</v>
+      </c>
+      <c r="P88">
+        <v>2.5</v>
+      </c>
+      <c r="Q88">
+        <v>15</v>
+      </c>
+      <c r="R88">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="S88">
+        <v>13</v>
+      </c>
+      <c r="U88">
+        <v>2.6</v>
+      </c>
+      <c r="V88">
+        <v>13</v>
+      </c>
+      <c r="W88">
+        <v>0.82</v>
+      </c>
+      <c r="X88">
+        <v>11</v>
+      </c>
+      <c r="Z88">
+        <v>5.4</v>
+      </c>
+      <c r="AA88">
+        <v>27</v>
+      </c>
+      <c r="AB88">
+        <v>0.82</v>
+      </c>
+      <c r="AC88">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89" spans="1:29">
+      <c r="A89">
+        <v>1.73</v>
+      </c>
+      <c r="B89">
+        <v>95</v>
+      </c>
+      <c r="C89">
+        <v>0.76</v>
+      </c>
+      <c r="D89">
+        <v>73</v>
+      </c>
+      <c r="F89">
+        <v>1.35</v>
+      </c>
+      <c r="G89">
+        <v>69</v>
+      </c>
+      <c r="H89">
+        <v>0.8</v>
+      </c>
+      <c r="I89">
+        <v>68</v>
+      </c>
+      <c r="K89">
+        <v>1.78</v>
+      </c>
+      <c r="L89">
+        <v>87</v>
+      </c>
+      <c r="M89">
+        <v>0.95</v>
+      </c>
+      <c r="N89">
+        <v>62</v>
+      </c>
+      <c r="P89">
+        <v>1.36</v>
+      </c>
+      <c r="Q89">
+        <v>75</v>
+      </c>
+      <c r="R89">
+        <v>0.91</v>
+      </c>
+      <c r="S89">
+        <v>69</v>
+      </c>
+      <c r="U89">
+        <v>1.63</v>
+      </c>
+      <c r="V89">
+        <v>88</v>
+      </c>
+      <c r="W89">
+        <v>0.8</v>
+      </c>
+      <c r="X89">
+        <v>71</v>
+      </c>
+      <c r="Z89">
+        <v>1.39</v>
+      </c>
+      <c r="AA89">
+        <v>82</v>
+      </c>
+      <c r="AB89">
+        <v>0.87</v>
+      </c>
+      <c r="AC89">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="90" spans="1:29">
+      <c r="A90">
+        <v>2</v>
+      </c>
+      <c r="B90">
+        <v>28</v>
+      </c>
+      <c r="C90">
+        <v>0.76</v>
+      </c>
+      <c r="D90">
+        <v>21</v>
+      </c>
+      <c r="F90">
+        <v>1.64</v>
+      </c>
+      <c r="G90">
+        <v>23</v>
+      </c>
+      <c r="H90">
+        <v>0.57</v>
+      </c>
+      <c r="I90">
+        <v>24</v>
+      </c>
+      <c r="K90">
+        <v>1.85</v>
+      </c>
+      <c r="L90">
+        <v>24</v>
+      </c>
+      <c r="M90">
+        <v>0.68</v>
+      </c>
+      <c r="N90">
+        <v>21</v>
+      </c>
+      <c r="P90">
+        <v>2.08</v>
+      </c>
+      <c r="Q90">
+        <v>25</v>
+      </c>
+      <c r="R90">
+        <v>0.87</v>
+      </c>
+      <c r="S90">
+        <v>18</v>
+      </c>
+      <c r="U90">
+        <v>2</v>
+      </c>
+      <c r="V90">
+        <v>28</v>
+      </c>
+      <c r="W90">
+        <v>0.57</v>
+      </c>
+      <c r="X90">
+        <v>24</v>
+      </c>
+      <c r="Z90">
+        <v>2.18</v>
+      </c>
+      <c r="AA90">
+        <v>24</v>
+      </c>
+      <c r="AB90">
+        <v>0.76</v>
+      </c>
+      <c r="AC90">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="93" spans="1:29">
+      <c r="A93" t="s">
+        <v>12</v>
+      </c>
+      <c r="C93" t="s">
+        <v>1</v>
+      </c>
+      <c r="F93" t="s">
+        <v>12</v>
+      </c>
+      <c r="H93" t="s">
+        <v>13</v>
+      </c>
+      <c r="K93" t="s">
+        <v>12</v>
+      </c>
+      <c r="M93" t="s">
+        <v>14</v>
+      </c>
+      <c r="P93" t="s">
+        <v>12</v>
+      </c>
+      <c r="R93" t="s">
+        <v>15</v>
+      </c>
+      <c r="U93" t="s">
+        <v>12</v>
+      </c>
+      <c r="W93" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z93" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB93" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="94" spans="1:29">
+      <c r="A94">
+        <v>1.81</v>
+      </c>
+      <c r="B94">
+        <v>29</v>
+      </c>
+      <c r="C94">
+        <v>0.88</v>
+      </c>
+      <c r="D94">
+        <v>21</v>
+      </c>
+      <c r="F94">
+        <v>1.39</v>
+      </c>
+      <c r="G94">
+        <v>25</v>
+      </c>
+      <c r="H94">
+        <v>0.6</v>
+      </c>
+      <c r="I94">
+        <v>27</v>
+      </c>
+      <c r="K94">
+        <v>1.42</v>
+      </c>
+      <c r="L94">
+        <v>27</v>
+      </c>
+      <c r="M94">
+        <v>0.88</v>
+      </c>
+      <c r="N94">
+        <v>24</v>
+      </c>
+      <c r="P94">
+        <v>1.76</v>
+      </c>
+      <c r="Q94">
+        <v>30</v>
+      </c>
+      <c r="R94">
+        <v>0.88</v>
+      </c>
+      <c r="S94">
+        <v>22</v>
+      </c>
+      <c r="U94">
+        <v>1.64</v>
+      </c>
+      <c r="V94">
+        <v>36</v>
+      </c>
+      <c r="W94">
+        <v>0.71</v>
+      </c>
+      <c r="X94">
+        <v>29</v>
+      </c>
+      <c r="Z94">
+        <v>1.76</v>
+      </c>
+      <c r="AA94">
+        <v>30</v>
+      </c>
+      <c r="AB94">
+        <v>0.88</v>
+      </c>
+      <c r="AC94">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="95" spans="1:29">
+      <c r="A95">
+        <v>1.68</v>
+      </c>
+      <c r="B95">
+        <v>32</v>
+      </c>
+      <c r="C95">
+        <v>0.73</v>
+      </c>
+      <c r="D95">
+        <v>25</v>
+      </c>
+      <c r="F95">
+        <v>1.68</v>
+      </c>
+      <c r="G95">
+        <v>37</v>
+      </c>
+      <c r="H95">
+        <v>0.48</v>
+      </c>
+      <c r="I95">
+        <v>32</v>
+      </c>
+      <c r="K95">
+        <v>1.47</v>
+      </c>
+      <c r="L95">
+        <v>28</v>
+      </c>
+      <c r="M95">
+        <v>0.65</v>
+      </c>
+      <c r="N95">
+        <v>26</v>
+      </c>
+      <c r="P95">
+        <v>1.57</v>
+      </c>
+      <c r="Q95">
+        <v>33</v>
+      </c>
+      <c r="R95">
+        <v>0.58</v>
+      </c>
+      <c r="S95">
+        <v>29</v>
+      </c>
+      <c r="U95">
+        <v>1.47</v>
+      </c>
+      <c r="V95">
+        <v>25</v>
+      </c>
+      <c r="W95">
+        <v>0.85</v>
+      </c>
+      <c r="X95">
+        <v>22</v>
+      </c>
+      <c r="Z95">
+        <v>1.65</v>
+      </c>
+      <c r="AA95">
+        <v>33</v>
+      </c>
+      <c r="AB95">
+        <v>0.65</v>
+      </c>
+      <c r="AC95">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="96" spans="1:29">
+      <c r="A96">
+        <v>2</v>
+      </c>
+      <c r="B96">
+        <v>12</v>
+      </c>
+      <c r="C96">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="D96">
+        <v>13</v>
+      </c>
+      <c r="F96">
+        <v>4.5</v>
+      </c>
+      <c r="G96">
+        <v>27</v>
+      </c>
+      <c r="H96">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="I96">
+        <v>13</v>
+      </c>
+      <c r="K96">
+        <v>2.6</v>
+      </c>
+      <c r="L96">
+        <v>13</v>
+      </c>
+      <c r="M96">
+        <v>0.82</v>
+      </c>
+      <c r="N96">
+        <v>11</v>
+      </c>
+      <c r="P96">
+        <v>2.6</v>
+      </c>
+      <c r="Q96">
+        <v>13</v>
+      </c>
+      <c r="R96">
+        <v>0.82</v>
+      </c>
+      <c r="S96">
+        <v>11</v>
+      </c>
+      <c r="U96">
+        <v>5.6</v>
+      </c>
+      <c r="V96">
+        <v>28</v>
+      </c>
+      <c r="W96">
+        <v>0.82</v>
+      </c>
+      <c r="X96">
+        <v>11</v>
+      </c>
+      <c r="Z96">
+        <v>6.6</v>
+      </c>
+      <c r="AA96">
+        <v>33</v>
+      </c>
+      <c r="AB96">
+        <v>0.82</v>
+      </c>
+      <c r="AC96">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="97" spans="1:29">
+      <c r="A97">
+        <v>1.37</v>
+      </c>
+      <c r="B97">
+        <v>78</v>
+      </c>
+      <c r="C97">
+        <v>0.95</v>
+      </c>
+      <c r="D97">
+        <v>70</v>
+      </c>
+      <c r="F97">
+        <v>1.58</v>
+      </c>
+      <c r="G97">
+        <v>104</v>
+      </c>
+      <c r="H97">
+        <v>0.95</v>
+      </c>
+      <c r="I97">
+        <v>79</v>
+      </c>
+      <c r="K97">
+        <v>1.76</v>
+      </c>
+      <c r="L97">
+        <v>97</v>
+      </c>
+      <c r="M97">
+        <v>0.95</v>
+      </c>
+      <c r="N97">
+        <v>68</v>
+      </c>
+      <c r="P97">
+        <v>1.78</v>
+      </c>
+      <c r="Q97">
+        <v>89</v>
+      </c>
+      <c r="R97">
+        <v>0.95</v>
+      </c>
+      <c r="S97">
+        <v>63</v>
+      </c>
+      <c r="U97">
+        <v>1.58</v>
+      </c>
+      <c r="V97">
+        <v>144</v>
+      </c>
+      <c r="W97">
+        <v>0.83</v>
+      </c>
+      <c r="X97">
+        <v>107</v>
+      </c>
+      <c r="Z97">
+        <v>1.94</v>
+      </c>
+      <c r="AA97">
+        <v>95</v>
+      </c>
+      <c r="AB97">
+        <v>1</v>
+      </c>
+      <c r="AC97">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="98" spans="1:29">
+      <c r="A98">
+        <v>1.59</v>
+      </c>
+      <c r="B98">
+        <v>27</v>
+      </c>
+      <c r="C98">
+        <v>0.62</v>
+      </c>
+      <c r="D98">
+        <v>26</v>
+      </c>
+      <c r="F98">
+        <v>2</v>
+      </c>
+      <c r="G98">
+        <v>22</v>
+      </c>
+      <c r="H98">
+        <v>0.62</v>
+      </c>
+      <c r="I98">
+        <v>20</v>
+      </c>
+      <c r="K98">
+        <v>2.5</v>
+      </c>
+      <c r="L98">
+        <v>20</v>
+      </c>
+      <c r="M98">
+        <v>0.87</v>
+      </c>
+      <c r="N98">
+        <v>14</v>
+      </c>
+      <c r="P98">
+        <v>1.86</v>
+      </c>
+      <c r="Q98">
+        <v>26</v>
+      </c>
+      <c r="R98">
+        <v>0.87</v>
+      </c>
+      <c r="S98">
+        <v>20</v>
+      </c>
+      <c r="U98">
+        <v>1.92</v>
+      </c>
+      <c r="V98">
+        <v>23</v>
+      </c>
+      <c r="W98">
+        <v>0.87</v>
+      </c>
+      <c r="X98">
+        <v>18</v>
+      </c>
+      <c r="Z98">
+        <v>1.62</v>
+      </c>
+      <c r="AA98">
+        <v>21</v>
+      </c>
+      <c r="AB98">
+        <v>0.76</v>
+      </c>
+      <c r="AC98">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>